<commit_message>
Update ignored enzyme list during optimization
</commit_message>
<xml_diff>
--- a/constant_enzymes.xlsx
+++ b/constant_enzymes.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://livelancsac-my.sharepoint.com/personal/vijayak2_lancaster_ac_uk/Documents/Code/C3-metabolic-and-leaf-model-svijayakumar_dev/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="27" documentId="8_{36A319C0-1870-40C2-A2FF-C08DCBFF010B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9FF51894-0839-4827-996D-22829766D7D3}"/>
+  <xr:revisionPtr revIDLastSave="46" documentId="8_{36A319C0-1870-40C2-A2FF-C08DCBFF010B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8839E0BF-05D0-4D75-BEA2-A8FA082C68E0}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" activeTab="1" xr2:uid="{74C4BDBC-9D23-4FDF-A4DC-7D8D1127E9B2}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="161" uniqueCount="64">
   <si>
     <t>Ci</t>
   </si>
@@ -214,6 +214,21 @@
   </si>
   <si>
     <t>Suggested</t>
+  </si>
+  <si>
+    <t>New</t>
+  </si>
+  <si>
+    <t>Transketolase</t>
+  </si>
+  <si>
+    <t>Fructose-bisphosphatase</t>
+  </si>
+  <si>
+    <t>1:6, 8,10,13:19</t>
+  </si>
+  <si>
+    <t>New Eio vector includes rows</t>
   </si>
 </sst>
 </file>
@@ -250,7 +265,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -272,6 +287,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="6" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -303,7 +324,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -333,6 +354,18 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -348,6 +381,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -649,8 +686,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B3246EEB-B0FD-423F-A1D3-4E791E88BFD6}">
   <dimension ref="A1:C29"/>
   <sheetViews>
-    <sheetView topLeftCell="A6" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4:C29"/>
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -717,30 +754,30 @@
         <v>10</v>
       </c>
     </row>
-    <row r="8" spans="1:3" ht="63" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:3" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A8" s="1"/>
       <c r="B8" s="4" t="s">
-        <v>11</v>
+        <v>61</v>
       </c>
       <c r="C8" s="2" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="9" spans="1:3" ht="31.8" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:3" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A9" s="1"/>
       <c r="B9" s="4" t="s">
-        <v>13</v>
+        <v>60</v>
       </c>
       <c r="C9" s="2" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="10" spans="1:3" ht="63" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="1"/>
-      <c r="B10" s="4" t="s">
+      <c r="A10" s="11"/>
+      <c r="B10" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="C10" s="2" t="s">
+      <c r="C10" s="13" t="s">
         <v>15</v>
       </c>
     </row>
@@ -754,11 +791,11 @@
       </c>
     </row>
     <row r="12" spans="1:3" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A12" s="1"/>
-      <c r="B12" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="C12" s="2" t="s">
+      <c r="A12" s="11"/>
+      <c r="B12" s="12" t="s">
+        <v>60</v>
+      </c>
+      <c r="C12" s="13" t="s">
         <v>18</v>
       </c>
     </row>
@@ -772,11 +809,11 @@
       </c>
     </row>
     <row r="14" spans="1:3" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A14" s="1"/>
-      <c r="B14" s="4" t="s">
+      <c r="A14" s="11"/>
+      <c r="B14" s="12" t="s">
         <v>21</v>
       </c>
-      <c r="C14" s="2" t="s">
+      <c r="C14" s="13" t="s">
         <v>22</v>
       </c>
     </row>
@@ -939,23 +976,33 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1D627708-668C-4C91-979B-6B85198DB793}">
-  <dimension ref="A1:D28"/>
+  <dimension ref="A1:H28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H3" sqref="H3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="4" max="4" width="33.44140625" customWidth="1"/>
+    <col min="8" max="8" width="30" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B1" t="s">
         <v>54</v>
       </c>
       <c r="D1" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="E1" t="s">
+        <v>59</v>
+      </c>
+      <c r="H1" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" ht="47.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>1</v>
       </c>
@@ -965,8 +1012,20 @@
       <c r="C2" s="2" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" ht="63" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="E2">
+        <v>1</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="H2" s="14" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" ht="63" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>2</v>
       </c>
@@ -976,8 +1035,17 @@
       <c r="C3" s="2" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" ht="125.4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="E3">
+        <v>2</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" ht="125.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>3</v>
       </c>
@@ -987,8 +1055,17 @@
       <c r="C4" s="2" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" ht="63" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="E4">
+        <v>3</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" ht="63" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>4</v>
       </c>
@@ -998,8 +1075,17 @@
       <c r="C5" s="2" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" ht="63" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="E5">
+        <v>4</v>
+      </c>
+      <c r="F5" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="G5" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" ht="63" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A6">
         <v>5</v>
       </c>
@@ -1009,8 +1095,17 @@
       <c r="C6" s="2" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" ht="31.8" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="E6">
+        <v>5</v>
+      </c>
+      <c r="F6" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="G6" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" ht="31.8" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A7">
         <v>6</v>
       </c>
@@ -1020,8 +1115,17 @@
       <c r="C7" s="2" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" ht="63" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="E7">
+        <v>6</v>
+      </c>
+      <c r="F7" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="G7" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" ht="63" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A8">
         <v>7</v>
       </c>
@@ -1034,8 +1138,17 @@
       <c r="D8" s="10" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="9" spans="1:4" ht="63" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="E8">
+        <v>7</v>
+      </c>
+      <c r="F8" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="G8" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" ht="63" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A9">
         <v>8</v>
       </c>
@@ -1045,8 +1158,17 @@
       <c r="C9" s="2" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="10" spans="1:4" ht="31.8" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="E9">
+        <v>8</v>
+      </c>
+      <c r="F9" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="G9" s="2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" ht="78.599999999999994" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A10">
         <v>9</v>
       </c>
@@ -1059,8 +1181,17 @@
       <c r="D10" s="10" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="11" spans="1:4" ht="47.4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="E10">
+        <v>9</v>
+      </c>
+      <c r="F10" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="G10" s="2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" ht="47.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A11">
         <v>10</v>
       </c>
@@ -1070,8 +1201,17 @@
       <c r="C11" s="2" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="12" spans="1:4" ht="109.8" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="E11">
+        <v>10</v>
+      </c>
+      <c r="F11" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="G11" s="2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" ht="125.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A12">
         <v>11</v>
       </c>
@@ -1084,8 +1224,17 @@
       <c r="D12" s="10" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="13" spans="1:4" ht="47.4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="E12">
+        <v>11</v>
+      </c>
+      <c r="F12" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="G12" s="2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" ht="78.599999999999994" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A13">
         <v>12</v>
       </c>
@@ -1098,8 +1247,17 @@
       <c r="D13" s="10" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="14" spans="1:4" ht="78.599999999999994" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="E13">
+        <v>12</v>
+      </c>
+      <c r="F13" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="G13" s="2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" ht="78.599999999999994" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A14">
         <v>13</v>
       </c>
@@ -1109,8 +1267,17 @@
       <c r="C14" s="2" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="15" spans="1:4" ht="31.8" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="E14">
+        <v>13</v>
+      </c>
+      <c r="F14" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="G14" s="2" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" ht="47.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A15">
         <v>14</v>
       </c>
@@ -1120,8 +1287,17 @@
       <c r="C15" s="2" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="16" spans="1:4" ht="125.4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="E15">
+        <v>14</v>
+      </c>
+      <c r="F15" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="G15" s="2" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" ht="125.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A16">
         <v>15</v>
       </c>
@@ -1130,6 +1306,15 @@
       </c>
       <c r="C16" s="2" t="s">
         <v>31</v>
+      </c>
+      <c r="E16">
+        <v>15</v>
+      </c>
+      <c r="F16" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="G16" s="2" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="78.599999999999994" thickBot="1" x14ac:dyDescent="0.35">

</xml_diff>